<commit_message>
update into console file
</commit_message>
<xml_diff>
--- a/console/Elastic-Compute/Virtual-Machine/common/errorMsg.xlsx
+++ b/console/Elastic-Compute/Virtual-Machine/common/errorMsg.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,13 +16,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>internal_wrong</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>内部错误</t>
+    <t>Internal Error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内部错误</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -30,7 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +57,19 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -78,12 +105,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -125,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -160,7 +190,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,19 +399,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="14.875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -395,7 +434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
@@ -408,7 +449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>

</xml_diff>